<commit_message>
finishing initial review of PacIOOS added some processing scripts and configs reprocessed output data files
</commit_message>
<xml_diff>
--- a/2020/data/processed/PacIOOS.xlsx
+++ b/2020/data/processed/PacIOOS.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="174">
   <si>
     <t>RA</t>
   </si>
@@ -684,6 +684,12 @@
   <si>
     <t>no obs for 2020 https://pae-paha.pacioos.hawaii.edu/erddap/tabledap/AWS-CRRF.html</t>
   </si>
+  <si>
+    <t>can't find station information via pacioos or IOOS Catalog.</t>
+  </si>
+  <si>
+    <t>can't find station information via pacioos or IOOS Catalog. Related to NS06 or pp02? http://oos.soest.hawaii.edu/erddap/search/index.html?page=1&amp;itemsPerPage=1000&amp;searchFor=pohnpei</t>
+  </si>
 </sst>
 </file>
 
@@ -1309,13 +1315,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1004"/>
+  <dimension ref="A1:V1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.69921875" defaultRowHeight="14.4"/>
@@ -2870,43 +2876,43 @@
         <v>35</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="C27" s="28" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="46">
-        <v>6.9866000000000001</v>
-      </c>
-      <c r="G27" s="46">
-        <v>158.22102000000001</v>
+      <c r="F27" s="29">
+        <v>21.2638</v>
+      </c>
+      <c r="G27" s="29">
+        <v>-157.76349999999999</v>
       </c>
       <c r="H27" s="29" t="s">
         <v>39</v>
       </c>
       <c r="I27" s="30">
-        <v>43443</v>
-      </c>
-      <c r="J27" s="44" t="s">
-        <v>62</v>
+        <v>43685</v>
+      </c>
+      <c r="J27" s="28" t="s">
+        <v>40</v>
       </c>
       <c r="K27" s="28" t="s">
-        <v>35</v>
+        <v>160</v>
       </c>
       <c r="L27" s="28" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="M27" s="28" t="s">
         <v>35</v>
       </c>
       <c r="N27" s="28" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="O27" s="28" t="s">
         <v>35</v>
@@ -2917,54 +2923,56 @@
       <c r="Q27" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="R27" s="28"/>
+      <c r="R27" s="28" t="s">
+        <v>154</v>
+      </c>
       <c r="S27" s="32"/>
       <c r="T27" s="32"/>
       <c r="U27" s="32"/>
       <c r="V27" s="32"/>
     </row>
     <row r="28" spans="1:22" s="33" customFormat="1" ht="27" customHeight="1">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="44" t="s">
-        <v>156</v>
+      <c r="B28" s="28" t="s">
+        <v>131</v>
       </c>
       <c r="C28" s="28" t="s">
         <v>37</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="46">
-        <v>7.52278</v>
-      </c>
-      <c r="G28" s="46">
-        <v>134.50138999999999</v>
+      <c r="F28" s="29">
+        <v>21.275860000000002</v>
+      </c>
+      <c r="G28" s="29">
+        <v>-157.7474</v>
       </c>
       <c r="H28" s="29" t="s">
         <v>39</v>
       </c>
       <c r="I28" s="30">
-        <v>43814</v>
+        <v>43685</v>
       </c>
       <c r="J28" s="28" t="s">
         <v>40</v>
       </c>
       <c r="K28" s="28" t="s">
-        <v>35</v>
+        <v>160</v>
       </c>
       <c r="L28" s="28" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="M28" s="28" t="s">
         <v>35</v>
       </c>
       <c r="N28" s="28" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="O28" s="28" t="s">
         <v>35</v>
@@ -2983,623 +2991,491 @@
       <c r="U28" s="32"/>
       <c r="V28" s="32"/>
     </row>
-    <row r="29" spans="1:22" s="50" customFormat="1" ht="54" customHeight="1">
-      <c r="A29" s="45" t="s">
+    <row r="29" spans="1:22" s="33" customFormat="1" ht="25.95" customHeight="1">
+      <c r="A29" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="44" t="s">
-        <v>158</v>
-      </c>
-      <c r="C29" s="44" t="s">
+      <c r="B29" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D29" s="44" t="s">
-        <v>159</v>
-      </c>
-      <c r="E29" s="44" t="s">
+      <c r="D29" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="68">
-        <v>20.791260000000001</v>
-      </c>
-      <c r="G29" s="68">
-        <v>-156.51127</v>
-      </c>
-      <c r="H29" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="I29" s="47">
-        <v>44044</v>
-      </c>
-      <c r="J29" s="44" t="s">
+      <c r="F29" s="29">
+        <v>21.27449</v>
+      </c>
+      <c r="G29" s="29">
+        <v>-157.71469999999999</v>
+      </c>
+      <c r="H29" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="30">
+        <v>43685</v>
+      </c>
+      <c r="J29" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="K29" s="44" t="s">
+      <c r="K29" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="M29" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="L29" s="44" t="s">
+      <c r="N29" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O29" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="P29" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q29" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="R29" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="S29" s="32"/>
+      <c r="T29" s="32"/>
+      <c r="U29" s="32"/>
+      <c r="V29" s="32"/>
+    </row>
+    <row r="30" spans="1:22" ht="46.95" customHeight="1">
+      <c r="A30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="28">
+        <v>51045</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="21">
+        <v>19.734200000000001</v>
+      </c>
+      <c r="G30" s="21">
+        <v>-155.08170000000001</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I30" s="15">
+        <v>40474</v>
+      </c>
+      <c r="J30" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M29" s="44" t="s">
+      <c r="M30" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="N29" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="O29" s="44" t="s">
+      <c r="N30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O30" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="P29" s="44" t="s">
+      <c r="P30" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q29" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="R29" s="44" t="s">
-        <v>154</v>
-      </c>
-      <c r="S29" s="49"/>
-      <c r="T29" s="49"/>
-      <c r="U29" s="49"/>
-      <c r="V29" s="49"/>
-    </row>
-    <row r="30" spans="1:22" s="33" customFormat="1" ht="28.05" customHeight="1">
-      <c r="A30" s="28" t="s">
+      <c r="Q30" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="R30" s="41"/>
+      <c r="S30" s="17"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="17"/>
+      <c r="V30" s="17"/>
+    </row>
+    <row r="31" spans="1:22" ht="39" customHeight="1">
+      <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="C30" s="28" t="s">
+      <c r="B31" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" s="28">
+        <v>51046</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="25">
+        <v>20.024100000000001</v>
+      </c>
+      <c r="G31" s="25">
+        <v>-155.82849999999999</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I31" s="15">
+        <v>43168</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N31" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P31" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q31" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="R31" s="35"/>
+      <c r="S31" s="17"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="17"/>
+      <c r="V31" s="17"/>
+    </row>
+    <row r="32" spans="1:22" ht="58.95" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="28">
+        <v>51043</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" s="14">
+        <v>21.288699999999999</v>
+      </c>
+      <c r="G32" s="14">
+        <v>-157.86500000000001</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" s="15">
+        <v>39667</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="N32" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O32" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q32" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="R32" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="S32" s="17"/>
+      <c r="T32" s="17"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="17"/>
+    </row>
+    <row r="33" spans="1:22" s="33" customFormat="1" ht="58.05" customHeight="1">
+      <c r="A33" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="28">
+        <v>51042</v>
+      </c>
+      <c r="D33" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="F33" s="29">
+        <v>21.279900000000001</v>
+      </c>
+      <c r="G33" s="29">
+        <v>-157.84800000000001</v>
+      </c>
+      <c r="H33" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I33" s="30">
+        <v>39667</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="L33" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="M33" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="N33" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O33" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="P33" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q33" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="R33" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
+      <c r="U33" s="32"/>
+      <c r="V33" s="32"/>
+    </row>
+    <row r="34" spans="1:22" s="33" customFormat="1" ht="61.05" customHeight="1">
+      <c r="A34" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D30" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="F30" s="29">
-        <v>21.2638</v>
-      </c>
-      <c r="G30" s="29">
-        <v>-157.76349999999999</v>
-      </c>
-      <c r="H30" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="30">
-        <v>43685</v>
-      </c>
-      <c r="J30" s="28" t="s">
+      <c r="D34" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="29">
+        <v>-14.3645</v>
+      </c>
+      <c r="G34" s="29">
+        <v>-170.7629</v>
+      </c>
+      <c r="H34" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34" s="51">
+        <v>43605</v>
+      </c>
+      <c r="J34" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="K30" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="L30" s="28" t="s">
+      <c r="K34" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="L34" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="M30" s="28" t="s">
+      <c r="M34" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="N30" s="28" t="s">
+      <c r="N34" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="O30" s="28" t="s">
+      <c r="O34" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="P30" s="28" t="s">
+      <c r="P34" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="Q30" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="R30" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="S30" s="32"/>
-      <c r="T30" s="32"/>
-      <c r="U30" s="32"/>
-      <c r="V30" s="32"/>
-    </row>
-    <row r="31" spans="1:22" s="33" customFormat="1" ht="27" customHeight="1">
-      <c r="A31" s="28" t="s">
+      <c r="Q34" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="R34" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="28"/>
+      <c r="V34" s="28"/>
+    </row>
+    <row r="35" spans="1:22" s="49" customFormat="1" ht="28.8">
+      <c r="A35" s="68" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" s="28" t="s">
+      <c r="B35" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="F31" s="29">
-        <v>21.275860000000002</v>
-      </c>
-      <c r="G31" s="29">
-        <v>-157.7474</v>
-      </c>
-      <c r="H31" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="I31" s="30">
-        <v>43685</v>
-      </c>
-      <c r="J31" s="28" t="s">
+      <c r="D35" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="F35" s="46">
+        <v>21.46</v>
+      </c>
+      <c r="G35" s="46">
+        <v>-157.80000000000001</v>
+      </c>
+      <c r="H35" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" s="47">
+        <v>39609</v>
+      </c>
+      <c r="J35" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="K31" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="L31" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="M31" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="N31" s="28" t="s">
+      <c r="K35" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="L35" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="M35" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="N35" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="O31" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="P31" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q31" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="R31" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="S31" s="32"/>
-      <c r="T31" s="32"/>
-      <c r="U31" s="32"/>
-      <c r="V31" s="32"/>
-    </row>
-    <row r="32" spans="1:22" s="33" customFormat="1" ht="25.95" customHeight="1">
-      <c r="A32" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="C32" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="F32" s="29">
-        <v>21.27449</v>
-      </c>
-      <c r="G32" s="29">
-        <v>-157.71469999999999</v>
-      </c>
-      <c r="H32" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32" s="30">
-        <v>43685</v>
-      </c>
-      <c r="J32" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="K32" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="L32" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="M32" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="N32" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="O32" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="P32" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q32" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="R32" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="S32" s="32"/>
-      <c r="T32" s="32"/>
-      <c r="U32" s="32"/>
-      <c r="V32" s="32"/>
-    </row>
-    <row r="33" spans="1:22" ht="46.95" customHeight="1">
-      <c r="A33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C33" s="28">
-        <v>51045</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F33" s="21">
-        <v>19.734200000000001</v>
-      </c>
-      <c r="G33" s="21">
-        <v>-155.08170000000001</v>
-      </c>
-      <c r="H33" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="I33" s="15">
-        <v>40474</v>
-      </c>
-      <c r="J33" s="35" t="s">
-        <v>40</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N33" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P33" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q33" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="R33" s="41"/>
-      <c r="S33" s="17"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="17"/>
-      <c r="V33" s="17"/>
-    </row>
-    <row r="34" spans="1:22" ht="39" customHeight="1">
-      <c r="A34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C34" s="28">
-        <v>51046</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="E34" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="F34" s="25">
-        <v>20.024100000000001</v>
-      </c>
-      <c r="G34" s="25">
-        <v>-155.82849999999999</v>
-      </c>
-      <c r="H34" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="I34" s="15">
-        <v>43168</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="M34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="N34" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="O34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q34" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="R34" s="35"/>
-      <c r="S34" s="17"/>
-      <c r="T34" s="17"/>
-      <c r="U34" s="17"/>
-      <c r="V34" s="17"/>
-    </row>
-    <row r="35" spans="1:22" ht="58.95" customHeight="1">
-      <c r="A35" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C35" s="28">
-        <v>51043</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E35" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="F35" s="14">
-        <v>21.288699999999999</v>
-      </c>
-      <c r="G35" s="14">
-        <v>-157.86500000000001</v>
-      </c>
-      <c r="H35" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="I35" s="15">
-        <v>39667</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="M35" s="5" t="s">
+      <c r="O35" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="N35" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="O35" s="5" t="s">
+      <c r="P35" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="P35" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q35" s="31" t="s">
+      <c r="Q35" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="R35" s="28" t="s">
+      <c r="R35" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="S35" s="17"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="17"/>
-      <c r="V35" s="17"/>
-    </row>
-    <row r="36" spans="1:22" s="33" customFormat="1" ht="58.05" customHeight="1">
-      <c r="A36" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C36" s="28">
-        <v>51042</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>136</v>
-      </c>
-      <c r="E36" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="F36" s="29">
-        <v>21.279900000000001</v>
-      </c>
-      <c r="G36" s="29">
-        <v>-157.84800000000001</v>
-      </c>
-      <c r="H36" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="I36" s="30">
-        <v>39667</v>
-      </c>
-      <c r="J36" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="K36" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="L36" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="M36" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="N36" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="O36" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="P36" s="28" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q36" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="R36" s="28" t="s">
-        <v>144</v>
-      </c>
-      <c r="S36" s="32"/>
-      <c r="T36" s="32"/>
-      <c r="U36" s="32"/>
-      <c r="V36" s="32"/>
-    </row>
-    <row r="37" spans="1:22" s="33" customFormat="1" ht="61.05" customHeight="1">
-      <c r="A37" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="C37" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>134</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="F37" s="29">
-        <v>-14.3645</v>
-      </c>
-      <c r="G37" s="29">
-        <v>-170.7629</v>
-      </c>
-      <c r="H37" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="I37" s="51">
-        <v>43605</v>
-      </c>
-      <c r="J37" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="K37" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="L37" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="M37" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="N37" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="O37" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="P37" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q37" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="R37" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="S37" s="28"/>
-      <c r="T37" s="28"/>
-      <c r="U37" s="28"/>
-      <c r="V37" s="28"/>
-    </row>
-    <row r="38" spans="1:22" s="49" customFormat="1" ht="28.8">
-      <c r="A38" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="44" t="s">
-        <v>168</v>
-      </c>
-      <c r="E38" s="69" t="s">
-        <v>143</v>
-      </c>
-      <c r="F38" s="46">
-        <v>21.46</v>
-      </c>
-      <c r="G38" s="46">
-        <v>-157.80000000000001</v>
-      </c>
-      <c r="H38" s="46" t="s">
-        <v>117</v>
-      </c>
-      <c r="I38" s="47">
-        <v>39609</v>
-      </c>
-      <c r="J38" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="K38" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="L38" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="M38" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="N38" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="O38" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="P38" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q38" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="R38" s="44" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="18"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="22"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
-      <c r="V39" s="5"/>
-    </row>
-    <row r="40" spans="1:22" ht="19.05" customHeight="1">
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+    </row>
+    <row r="37" spans="1:22" ht="19.05" customHeight="1">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="22"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="5"/>
+      <c r="U37" s="5"/>
+      <c r="V37" s="5"/>
+    </row>
+    <row r="38" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="5"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="5"/>
+      <c r="T38" s="5"/>
+      <c r="U38" s="5"/>
+      <c r="V38" s="5"/>
+    </row>
+    <row r="40" spans="1:22" ht="13.5" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -3616,7 +3492,7 @@
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
-      <c r="Q40" s="22"/>
+      <c r="Q40" s="5"/>
       <c r="R40" s="5"/>
       <c r="S40" s="5"/>
       <c r="T40" s="5"/>
@@ -3647,6 +3523,30 @@
       <c r="U41" s="5"/>
       <c r="V41" s="5"/>
     </row>
+    <row r="42" spans="1:22" ht="13.5" customHeight="1">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+      <c r="P42" s="5"/>
+      <c r="Q42" s="5"/>
+      <c r="R42" s="5"/>
+      <c r="S42" s="5"/>
+      <c r="T42" s="5"/>
+      <c r="U42" s="5"/>
+      <c r="V42" s="5"/>
+    </row>
     <row r="43" spans="1:22" ht="13.5" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
@@ -26552,7 +26452,6 @@
       <c r="F997" s="14"/>
       <c r="G997" s="14"/>
       <c r="H997" s="14"/>
-      <c r="I997" s="18"/>
       <c r="J997" s="5"/>
       <c r="K997" s="5"/>
       <c r="L997" s="5"/>
@@ -26576,7 +26475,6 @@
       <c r="F998" s="14"/>
       <c r="G998" s="14"/>
       <c r="H998" s="14"/>
-      <c r="I998" s="18"/>
       <c r="J998" s="5"/>
       <c r="K998" s="5"/>
       <c r="L998" s="5"/>
@@ -26600,7 +26498,6 @@
       <c r="F999" s="14"/>
       <c r="G999" s="14"/>
       <c r="H999" s="14"/>
-      <c r="I999" s="18"/>
       <c r="J999" s="5"/>
       <c r="K999" s="5"/>
       <c r="L999" s="5"/>
@@ -26661,75 +26558,6 @@
       <c r="U1001" s="5"/>
       <c r="V1001" s="5"/>
     </row>
-    <row r="1002" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A1002" s="5"/>
-      <c r="B1002" s="5"/>
-      <c r="C1002" s="5"/>
-      <c r="D1002" s="5"/>
-      <c r="E1002" s="5"/>
-      <c r="F1002" s="14"/>
-      <c r="G1002" s="14"/>
-      <c r="H1002" s="14"/>
-      <c r="J1002" s="5"/>
-      <c r="K1002" s="5"/>
-      <c r="L1002" s="5"/>
-      <c r="M1002" s="5"/>
-      <c r="N1002" s="5"/>
-      <c r="O1002" s="5"/>
-      <c r="P1002" s="5"/>
-      <c r="Q1002" s="5"/>
-      <c r="R1002" s="5"/>
-      <c r="S1002" s="5"/>
-      <c r="T1002" s="5"/>
-      <c r="U1002" s="5"/>
-      <c r="V1002" s="5"/>
-    </row>
-    <row r="1003" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A1003" s="5"/>
-      <c r="B1003" s="5"/>
-      <c r="C1003" s="5"/>
-      <c r="D1003" s="5"/>
-      <c r="E1003" s="5"/>
-      <c r="F1003" s="14"/>
-      <c r="G1003" s="14"/>
-      <c r="H1003" s="14"/>
-      <c r="J1003" s="5"/>
-      <c r="K1003" s="5"/>
-      <c r="L1003" s="5"/>
-      <c r="M1003" s="5"/>
-      <c r="N1003" s="5"/>
-      <c r="O1003" s="5"/>
-      <c r="P1003" s="5"/>
-      <c r="Q1003" s="5"/>
-      <c r="R1003" s="5"/>
-      <c r="S1003" s="5"/>
-      <c r="T1003" s="5"/>
-      <c r="U1003" s="5"/>
-      <c r="V1003" s="5"/>
-    </row>
-    <row r="1004" spans="1:22" ht="13.5" customHeight="1">
-      <c r="A1004" s="5"/>
-      <c r="B1004" s="5"/>
-      <c r="C1004" s="5"/>
-      <c r="D1004" s="5"/>
-      <c r="E1004" s="5"/>
-      <c r="F1004" s="14"/>
-      <c r="G1004" s="14"/>
-      <c r="H1004" s="14"/>
-      <c r="J1004" s="5"/>
-      <c r="K1004" s="5"/>
-      <c r="L1004" s="5"/>
-      <c r="M1004" s="5"/>
-      <c r="N1004" s="5"/>
-      <c r="O1004" s="5"/>
-      <c r="P1004" s="5"/>
-      <c r="Q1004" s="5"/>
-      <c r="R1004" s="5"/>
-      <c r="S1004" s="5"/>
-      <c r="T1004" s="5"/>
-      <c r="U1004" s="5"/>
-      <c r="V1004" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -26743,10 +26571,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -26992,6 +26820,190 @@
       <c r="T4" s="65"/>
       <c r="U4" s="65"/>
       <c r="V4" s="65"/>
+    </row>
+    <row r="5" spans="1:22" s="50" customFormat="1" ht="54" customHeight="1">
+      <c r="A5" s="45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="68">
+        <v>20.791260000000001</v>
+      </c>
+      <c r="G5" s="68">
+        <v>-156.51127</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="I5" s="47">
+        <v>44044</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="44" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="R5" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+    </row>
+    <row r="6" spans="1:22" s="33" customFormat="1" ht="27" customHeight="1">
+      <c r="A6" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="46">
+        <v>7.52278</v>
+      </c>
+      <c r="G6" s="46">
+        <v>134.50138999999999</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="30">
+        <v>43814</v>
+      </c>
+      <c r="J6" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="R6" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+    </row>
+    <row r="7" spans="1:22" s="33" customFormat="1" ht="28.05" customHeight="1">
+      <c r="A7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="46">
+        <v>6.9866000000000001</v>
+      </c>
+      <c r="G7" s="46">
+        <v>158.22102000000001</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="30">
+        <v>43443</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="R7" s="28"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="U7" s="32"/>
+      <c r="V7" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cleaning up script creating environment file writing raw inventory to kml file
</commit_message>
<xml_diff>
--- a/2020/data/processed/PacIOOS.xlsx
+++ b/2020/data/processed/PacIOOS.xlsx
@@ -5,16 +5,17 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\Documents\GitProjects\assetInventory\2020\data\processed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathew.Biddle\PycharmProjects\assetInventory\2020\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-96" yWindow="504" windowWidth="51204" windowHeight="26784"/>
   </bookViews>
   <sheets>
-    <sheet name="PacIOOS assets_2020" sheetId="3" r:id="rId1"/>
-    <sheet name="IOOS removed" sheetId="4" r:id="rId2"/>
-    <sheet name="Definitions" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="PacIOOS assets_2020" sheetId="3" r:id="rId2"/>
+    <sheet name="IOOS removed" sheetId="4" r:id="rId3"/>
+    <sheet name="Definitions" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ValidObservedVariables">#REF!</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="175">
   <si>
     <t>RA</t>
   </si>
@@ -690,6 +691,9 @@
   <si>
     <t>can't find station information via pacioos or IOOS Catalog. Related to NS06 or pp02? http://oos.soest.hawaii.edu/erddap/search/index.html?page=1&amp;itemsPerPage=1000&amp;searchFor=pohnpei</t>
   </si>
+  <si>
+    <t>sea_surface_wave_from_direction, sea_surface_wave_mean_period_from_variance_spectral_density_second_frequency_moment, sea_surface_wave_period_at_variance_spectral_density_maximum, sea_surface_wave_significant_height, sea_water_speed, sea_water_temperature, sea_water_to_direction</t>
+  </si>
 </sst>
 </file>
 
@@ -1025,9 +1029,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1070,6 +1071,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1315,13 +1317,1928 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="9" max="9" width="9.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2">
+        <v>21.433</v>
+      </c>
+      <c r="G2">
+        <v>-157.78630000000001</v>
+      </c>
+      <c r="H2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="69">
+        <v>38353</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3">
+        <v>21.296199999999999</v>
+      </c>
+      <c r="G3">
+        <v>-157.86869999999999</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="69">
+        <v>43691</v>
+      </c>
+      <c r="J3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" t="s">
+        <v>140</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" t="s">
+        <v>141</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>142</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>51202</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4">
+        <v>21.414999999999999</v>
+      </c>
+      <c r="G4">
+        <v>-157.67830000000001</v>
+      </c>
+      <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="69">
+        <v>36747</v>
+      </c>
+      <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O4" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>51201</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5">
+        <v>21.670500000000001</v>
+      </c>
+      <c r="G5">
+        <v>-158.1172</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="69">
+        <v>37240</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>52200</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6">
+        <v>13.354200000000001</v>
+      </c>
+      <c r="G6">
+        <v>144.78829999999999</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="69">
+        <v>37817</v>
+      </c>
+      <c r="J6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" t="s">
+        <v>55</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" t="s">
+        <v>49</v>
+      </c>
+      <c r="O6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7">
+        <v>52201</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7">
+        <v>7.0834999999999999</v>
+      </c>
+      <c r="G7">
+        <v>171.39179999999999</v>
+      </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="69">
+        <v>42494</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8">
+        <v>51205</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8">
+        <v>21.0182</v>
+      </c>
+      <c r="G8">
+        <v>-156.42519999999999</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="69">
+        <v>40880</v>
+      </c>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+      <c r="K8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" t="s">
+        <v>49</v>
+      </c>
+      <c r="O8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P8" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>57</v>
+      </c>
+      <c r="R8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>51206</v>
+      </c>
+      <c r="D9" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9">
+        <v>19.78</v>
+      </c>
+      <c r="G9">
+        <v>-154.97</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="69">
+        <v>40972</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" t="s">
+        <v>35</v>
+      </c>
+      <c r="L9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10">
+        <v>51209</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10">
+        <v>-14.2645</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="69">
+        <v>41935</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" t="s">
+        <v>49</v>
+      </c>
+      <c r="O10" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11">
+        <v>52202</v>
+      </c>
+      <c r="D11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11">
+        <v>13.6837</v>
+      </c>
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="69">
+        <v>41202</v>
+      </c>
+      <c r="J11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+      <c r="L11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>49</v>
+      </c>
+      <c r="O11" t="s">
+        <v>35</v>
+      </c>
+      <c r="P11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>57</v>
+      </c>
+      <c r="R11" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12">
+        <v>52211</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12">
+        <v>15.2685</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="69">
+        <v>41206</v>
+      </c>
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13">
+        <v>51207</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13">
+        <v>21.477499999999999</v>
+      </c>
+      <c r="G13">
+        <v>-157.7526</v>
+      </c>
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="69">
+        <v>41198</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" t="s">
+        <v>80</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O13" t="s">
+        <v>35</v>
+      </c>
+      <c r="P13" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14">
+        <v>51208</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14">
+        <v>22.284700000000001</v>
+      </c>
+      <c r="G14">
+        <v>-159.57419999999999</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="69">
+        <v>41549</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" t="s">
+        <v>49</v>
+      </c>
+      <c r="O14" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>57</v>
+      </c>
+      <c r="R14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15">
+        <v>51210</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15">
+        <v>21.477399999999999</v>
+      </c>
+      <c r="G15">
+        <v>-157.75579999999999</v>
+      </c>
+      <c r="H15" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="69">
+        <v>43034</v>
+      </c>
+      <c r="J15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" t="s">
+        <v>80</v>
+      </c>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16">
+        <v>51211</v>
+      </c>
+      <c r="D16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16">
+        <v>21.2974</v>
+      </c>
+      <c r="G16">
+        <v>-157.9589</v>
+      </c>
+      <c r="H16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="69">
+        <v>42892</v>
+      </c>
+      <c r="J16" t="s">
+        <v>40</v>
+      </c>
+      <c r="K16" t="s">
+        <v>35</v>
+      </c>
+      <c r="L16" t="s">
+        <v>55</v>
+      </c>
+      <c r="M16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" t="s">
+        <v>49</v>
+      </c>
+      <c r="O16" t="s">
+        <v>35</v>
+      </c>
+      <c r="P16" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17">
+        <v>51212</v>
+      </c>
+      <c r="D17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17">
+        <v>21.3233</v>
+      </c>
+      <c r="G17">
+        <v>-158.1497</v>
+      </c>
+      <c r="H17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="69">
+        <v>43251</v>
+      </c>
+      <c r="J17" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" t="s">
+        <v>55</v>
+      </c>
+      <c r="M17" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" t="s">
+        <v>49</v>
+      </c>
+      <c r="O17" t="s">
+        <v>35</v>
+      </c>
+      <c r="P17" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18">
+        <v>51213</v>
+      </c>
+      <c r="D18" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18">
+        <v>20.7502</v>
+      </c>
+      <c r="G18">
+        <v>-157.0034</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="69">
+        <v>43271</v>
+      </c>
+      <c r="J18" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" t="s">
+        <v>55</v>
+      </c>
+      <c r="M18" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" t="s">
+        <v>49</v>
+      </c>
+      <c r="O18" t="s">
+        <v>35</v>
+      </c>
+      <c r="P18" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19">
+        <v>21.28641</v>
+      </c>
+      <c r="G19">
+        <v>-157.84280000000001</v>
+      </c>
+      <c r="H19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="69">
+        <v>39657</v>
+      </c>
+      <c r="J19" t="s">
+        <v>40</v>
+      </c>
+      <c r="K19" t="s">
+        <v>35</v>
+      </c>
+      <c r="L19" t="s">
+        <v>55</v>
+      </c>
+      <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>49</v>
+      </c>
+      <c r="O19" t="s">
+        <v>35</v>
+      </c>
+      <c r="P19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20">
+        <v>21.280419999999999</v>
+      </c>
+      <c r="G20">
+        <v>-157.8381</v>
+      </c>
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="69">
+        <v>39828</v>
+      </c>
+      <c r="J20" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L20" t="s">
+        <v>55</v>
+      </c>
+      <c r="M20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" t="s">
+        <v>49</v>
+      </c>
+      <c r="O20" t="s">
+        <v>35</v>
+      </c>
+      <c r="P20" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E21" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21">
+        <v>-157.8228</v>
+      </c>
+      <c r="H21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="69">
+        <v>40081</v>
+      </c>
+      <c r="J21" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" t="s">
+        <v>35</v>
+      </c>
+      <c r="L21" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>49</v>
+      </c>
+      <c r="O21" t="s">
+        <v>35</v>
+      </c>
+      <c r="P21" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22">
+        <v>-14.2766</v>
+      </c>
+      <c r="G22">
+        <v>-170.6908</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="69">
+        <v>40337</v>
+      </c>
+      <c r="J22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K22" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" t="s">
+        <v>55</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>49</v>
+      </c>
+      <c r="O22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>95</v>
+      </c>
+      <c r="R22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" t="s">
+        <v>94</v>
+      </c>
+      <c r="F23">
+        <v>6.8736810000000004</v>
+      </c>
+      <c r="G23">
+        <v>158.22450000000001</v>
+      </c>
+      <c r="H23" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="69">
+        <v>40305</v>
+      </c>
+      <c r="J23" t="s">
+        <v>40</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23" t="s">
+        <v>55</v>
+      </c>
+      <c r="M23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" t="s">
+        <v>49</v>
+      </c>
+      <c r="O23" t="s">
+        <v>35</v>
+      </c>
+      <c r="P23" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>95</v>
+      </c>
+      <c r="R23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24">
+        <v>7.1059999999999999</v>
+      </c>
+      <c r="G24">
+        <v>171.37280000000001</v>
+      </c>
+      <c r="H24" t="s">
+        <v>39</v>
+      </c>
+      <c r="I24" s="69">
+        <v>40300</v>
+      </c>
+      <c r="J24" t="s">
+        <v>40</v>
+      </c>
+      <c r="K24" t="s">
+        <v>35</v>
+      </c>
+      <c r="L24" t="s">
+        <v>55</v>
+      </c>
+      <c r="M24" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" t="s">
+        <v>49</v>
+      </c>
+      <c r="O24" t="s">
+        <v>35</v>
+      </c>
+      <c r="P24" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>95</v>
+      </c>
+      <c r="R24" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C25" t="s">
+        <v>166</v>
+      </c>
+      <c r="D25" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25">
+        <v>21.280090000000001</v>
+      </c>
+      <c r="G25">
+        <v>-157.71100000000001</v>
+      </c>
+      <c r="H25" t="s">
+        <v>39</v>
+      </c>
+      <c r="I25" s="69">
+        <v>40693</v>
+      </c>
+      <c r="J25" t="s">
+        <v>40</v>
+      </c>
+      <c r="K25" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25" t="s">
+        <v>55</v>
+      </c>
+      <c r="M25" t="s">
+        <v>35</v>
+      </c>
+      <c r="N25" t="s">
+        <v>49</v>
+      </c>
+      <c r="O25" t="s">
+        <v>35</v>
+      </c>
+      <c r="P25" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26">
+        <v>20.731210000000001</v>
+      </c>
+      <c r="G26">
+        <v>-156.45500000000001</v>
+      </c>
+      <c r="H26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="69">
+        <v>41852</v>
+      </c>
+      <c r="J26" t="s">
+        <v>40</v>
+      </c>
+      <c r="K26" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26" t="s">
+        <v>55</v>
+      </c>
+      <c r="M26" t="s">
+        <v>35</v>
+      </c>
+      <c r="N26" t="s">
+        <v>49</v>
+      </c>
+      <c r="O26" t="s">
+        <v>35</v>
+      </c>
+      <c r="P26" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>95</v>
+      </c>
+      <c r="R26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>130</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27">
+        <v>21.2638</v>
+      </c>
+      <c r="G27">
+        <v>-157.76349999999999</v>
+      </c>
+      <c r="H27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="69">
+        <v>43685</v>
+      </c>
+      <c r="J27" t="s">
+        <v>40</v>
+      </c>
+      <c r="K27" t="s">
+        <v>160</v>
+      </c>
+      <c r="L27" t="s">
+        <v>80</v>
+      </c>
+      <c r="M27" t="s">
+        <v>35</v>
+      </c>
+      <c r="N27" t="s">
+        <v>49</v>
+      </c>
+      <c r="O27" t="s">
+        <v>35</v>
+      </c>
+      <c r="P27" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>95</v>
+      </c>
+      <c r="R27" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28">
+        <v>21.275860000000002</v>
+      </c>
+      <c r="G28">
+        <v>-157.7474</v>
+      </c>
+      <c r="H28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I28" s="69">
+        <v>43685</v>
+      </c>
+      <c r="J28" t="s">
+        <v>40</v>
+      </c>
+      <c r="K28" t="s">
+        <v>160</v>
+      </c>
+      <c r="L28" t="s">
+        <v>80</v>
+      </c>
+      <c r="M28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N28" t="s">
+        <v>49</v>
+      </c>
+      <c r="O28" t="s">
+        <v>35</v>
+      </c>
+      <c r="P28" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>95</v>
+      </c>
+      <c r="R28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29">
+        <v>21.27449</v>
+      </c>
+      <c r="G29">
+        <v>-157.71469999999999</v>
+      </c>
+      <c r="H29" t="s">
+        <v>39</v>
+      </c>
+      <c r="I29" s="69">
+        <v>43685</v>
+      </c>
+      <c r="J29" t="s">
+        <v>40</v>
+      </c>
+      <c r="K29" t="s">
+        <v>160</v>
+      </c>
+      <c r="L29" t="s">
+        <v>80</v>
+      </c>
+      <c r="M29" t="s">
+        <v>35</v>
+      </c>
+      <c r="N29" t="s">
+        <v>49</v>
+      </c>
+      <c r="O29" t="s">
+        <v>35</v>
+      </c>
+      <c r="P29" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>95</v>
+      </c>
+      <c r="R29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30">
+        <v>51045</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30">
+        <v>19.734200000000001</v>
+      </c>
+      <c r="G30">
+        <v>-155.08170000000001</v>
+      </c>
+      <c r="H30" t="s">
+        <v>117</v>
+      </c>
+      <c r="I30" s="69">
+        <v>40474</v>
+      </c>
+      <c r="J30" t="s">
+        <v>40</v>
+      </c>
+      <c r="K30" t="s">
+        <v>35</v>
+      </c>
+      <c r="L30" t="s">
+        <v>55</v>
+      </c>
+      <c r="M30" t="s">
+        <v>35</v>
+      </c>
+      <c r="N30" t="s">
+        <v>49</v>
+      </c>
+      <c r="O30" t="s">
+        <v>35</v>
+      </c>
+      <c r="P30" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31">
+        <v>51046</v>
+      </c>
+      <c r="D31" t="s">
+        <v>120</v>
+      </c>
+      <c r="E31" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31">
+        <v>20.024100000000001</v>
+      </c>
+      <c r="G31">
+        <v>-155.82849999999999</v>
+      </c>
+      <c r="H31" t="s">
+        <v>117</v>
+      </c>
+      <c r="I31" s="69">
+        <v>43168</v>
+      </c>
+      <c r="J31" t="s">
+        <v>40</v>
+      </c>
+      <c r="K31" t="s">
+        <v>122</v>
+      </c>
+      <c r="L31" t="s">
+        <v>55</v>
+      </c>
+      <c r="M31" t="s">
+        <v>35</v>
+      </c>
+      <c r="N31" t="s">
+        <v>49</v>
+      </c>
+      <c r="O31" t="s">
+        <v>35</v>
+      </c>
+      <c r="P31" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32">
+        <v>51043</v>
+      </c>
+      <c r="D32" t="s">
+        <v>124</v>
+      </c>
+      <c r="E32" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32">
+        <v>21.288699999999999</v>
+      </c>
+      <c r="G32">
+        <v>-157.86500000000001</v>
+      </c>
+      <c r="H32" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" s="69">
+        <v>39667</v>
+      </c>
+      <c r="J32" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" t="s">
+        <v>125</v>
+      </c>
+      <c r="L32" t="s">
+        <v>41</v>
+      </c>
+      <c r="M32" t="s">
+        <v>126</v>
+      </c>
+      <c r="N32" t="s">
+        <v>49</v>
+      </c>
+      <c r="O32" t="s">
+        <v>126</v>
+      </c>
+      <c r="P32" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>149</v>
+      </c>
+      <c r="R32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33">
+        <v>51042</v>
+      </c>
+      <c r="D33" t="s">
+        <v>136</v>
+      </c>
+      <c r="E33" t="s">
+        <v>143</v>
+      </c>
+      <c r="F33">
+        <v>21.279900000000001</v>
+      </c>
+      <c r="G33">
+        <v>-157.84800000000001</v>
+      </c>
+      <c r="H33" t="s">
+        <v>117</v>
+      </c>
+      <c r="I33" s="69">
+        <v>39667</v>
+      </c>
+      <c r="J33" t="s">
+        <v>40</v>
+      </c>
+      <c r="K33" t="s">
+        <v>125</v>
+      </c>
+      <c r="L33" t="s">
+        <v>41</v>
+      </c>
+      <c r="M33" t="s">
+        <v>126</v>
+      </c>
+      <c r="N33" t="s">
+        <v>49</v>
+      </c>
+      <c r="O33" t="s">
+        <v>126</v>
+      </c>
+      <c r="P33" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>149</v>
+      </c>
+      <c r="R33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34">
+        <v>-14.3645</v>
+      </c>
+      <c r="G34">
+        <v>-170.7629</v>
+      </c>
+      <c r="H34" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34" s="69">
+        <v>43605</v>
+      </c>
+      <c r="J34" t="s">
+        <v>40</v>
+      </c>
+      <c r="K34" t="s">
+        <v>125</v>
+      </c>
+      <c r="L34" t="s">
+        <v>80</v>
+      </c>
+      <c r="M34" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34" t="s">
+        <v>49</v>
+      </c>
+      <c r="O34" t="s">
+        <v>35</v>
+      </c>
+      <c r="P34" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>149</v>
+      </c>
+      <c r="R34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>167</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" t="s">
+        <v>143</v>
+      </c>
+      <c r="F35">
+        <v>21.46</v>
+      </c>
+      <c r="G35">
+        <v>-157.80000000000001</v>
+      </c>
+      <c r="H35" t="s">
+        <v>117</v>
+      </c>
+      <c r="I35" s="69">
+        <v>39609</v>
+      </c>
+      <c r="J35" t="s">
+        <v>40</v>
+      </c>
+      <c r="K35" t="s">
+        <v>125</v>
+      </c>
+      <c r="L35" t="s">
+        <v>41</v>
+      </c>
+      <c r="M35" t="s">
+        <v>126</v>
+      </c>
+      <c r="N35" t="s">
+        <v>49</v>
+      </c>
+      <c r="O35" t="s">
+        <v>126</v>
+      </c>
+      <c r="P35" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>149</v>
+      </c>
+      <c r="R35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection sqref="A1:R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.69921875" defaultRowHeight="14.4"/>
@@ -2406,7 +4323,7 @@
       <c r="B19" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="66" t="s">
         <v>163</v>
       </c>
       <c r="D19" s="5" t="s">
@@ -2464,7 +4381,7 @@
       <c r="B20" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C20" s="66" t="s">
         <v>164</v>
       </c>
       <c r="D20" s="5" t="s">
@@ -2522,7 +4439,7 @@
       <c r="B21" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="66" t="s">
         <v>165</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -2760,7 +4677,7 @@
       <c r="B25" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="67" t="s">
+      <c r="C25" s="66" t="s">
         <v>166</v>
       </c>
       <c r="D25" s="5" t="s">
@@ -3240,7 +5157,7 @@
       <c r="D33" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="E33" s="52" t="s">
+      <c r="E33" s="51" t="s">
         <v>143</v>
       </c>
       <c r="F33" s="29">
@@ -3312,7 +5229,7 @@
       <c r="H34" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="I34" s="51">
+      <c r="I34" s="30">
         <v>43605</v>
       </c>
       <c r="J34" s="28" t="s">
@@ -3348,7 +5265,7 @@
       <c r="V34" s="28"/>
     </row>
     <row r="35" spans="1:22" s="49" customFormat="1" ht="28.8">
-      <c r="A35" s="68" t="s">
+      <c r="A35" s="67" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="44" t="s">
@@ -3360,7 +5277,7 @@
       <c r="D35" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="E35" s="69" t="s">
+      <c r="E35" s="68" t="s">
         <v>143</v>
       </c>
       <c r="F35" s="46">
@@ -26569,7 +28486,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V7"/>
   <sheetViews>
@@ -26641,63 +28558,63 @@
       <c r="U1" s="13"/>
       <c r="V1" s="13"/>
     </row>
-    <row r="2" spans="1:22" s="59" customFormat="1" ht="34.049999999999997" customHeight="1">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:22" s="58" customFormat="1" ht="34.049999999999997" customHeight="1">
+      <c r="A2" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54">
+      <c r="E2" s="52"/>
+      <c r="F2" s="53">
         <v>7.2091500000000002</v>
       </c>
-      <c r="G2" s="54">
+      <c r="G2" s="53">
         <v>134.37100000000001</v>
       </c>
-      <c r="H2" s="55" t="s">
+      <c r="H2" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="56">
+      <c r="I2" s="55">
         <v>39141</v>
       </c>
-      <c r="J2" s="53" t="s">
+      <c r="J2" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53" t="s">
+      <c r="K2" s="52"/>
+      <c r="L2" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="53" t="s">
+      <c r="M2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="53" t="s">
+      <c r="N2" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="53" t="s">
+      <c r="O2" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="53" t="s">
+      <c r="P2" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="57" t="s">
+      <c r="Q2" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="53" t="s">
+      <c r="R2" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="58"/>
-      <c r="T2" s="58" t="s">
+      <c r="S2" s="57"/>
+      <c r="T2" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="U2" s="58"/>
-      <c r="V2" s="58"/>
+      <c r="U2" s="57"/>
+      <c r="V2" s="57"/>
     </row>
     <row r="3" spans="1:22" s="40" customFormat="1" ht="28.05" customHeight="1">
       <c r="A3" s="28" t="s">
@@ -26761,65 +28678,65 @@
       <c r="U3" s="39"/>
       <c r="V3" s="39"/>
     </row>
-    <row r="4" spans="1:22" s="66" customFormat="1" ht="28.05" customHeight="1">
-      <c r="A4" s="60" t="s">
+    <row r="4" spans="1:22" s="65" customFormat="1" ht="28.05" customHeight="1">
+      <c r="A4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="59" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="60" t="s">
+      <c r="E4" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="61">
+      <c r="F4" s="60">
         <v>21.2682</v>
       </c>
-      <c r="G4" s="61">
+      <c r="G4" s="60">
         <v>-157.77670000000001</v>
       </c>
-      <c r="H4" s="62" t="s">
+      <c r="H4" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="62">
         <v>43357</v>
       </c>
-      <c r="J4" s="60" t="s">
+      <c r="J4" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="60" t="s">
+      <c r="K4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="L4" s="60" t="s">
+      <c r="L4" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="M4" s="60" t="s">
+      <c r="M4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="N4" s="60" t="s">
+      <c r="N4" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="60" t="s">
+      <c r="O4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="60" t="s">
+      <c r="P4" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="64" t="s">
+      <c r="Q4" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="R4" s="60" t="s">
+      <c r="R4" s="59" t="s">
         <v>157</v>
       </c>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
-      <c r="U4" s="65"/>
-      <c r="V4" s="65"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
     </row>
     <row r="5" spans="1:22" s="50" customFormat="1" ht="54" customHeight="1">
       <c r="A5" s="45" t="s">
@@ -26837,10 +28754,10 @@
       <c r="E5" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="68">
+      <c r="F5" s="67">
         <v>20.791260000000001</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="67">
         <v>-156.51127</v>
       </c>
       <c r="H5" s="46" t="s">
@@ -27010,7 +28927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>

</xml_diff>